<commit_message>
adding example into the xlsx
</commit_message>
<xml_diff>
--- a/feature_xlsx/1.0.0-example_feature/1.0.0-example_feature.xlsx
+++ b/feature_xlsx/1.0.0-example_feature/1.0.0-example_feature.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nowpngs/Desktop/Programing/Personal/universal-feature-update/example_project/1.0.0-example_feature/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nowpngs/Desktop/Programing/Personal/universal-feature-update/feature_xlsx/1.0.0-example_feature/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB892A26-3A2C-D64A-99D0-CE92F53C76A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB9AAE5-DC64-B347-8D9D-BFFDAB733293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{DDFCAD63-2E02-1143-AAA5-04CC48EE4CF7}"/>
+    <workbookView xWindow="2760" yWindow="1540" windowWidth="28040" windowHeight="17440" xr2:uid="{DDFCAD63-2E02-1143-AAA5-04CC48EE4CF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Index</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>Commit SHA</t>
+  </si>
+  <si>
+    <t>git@github.com:Nowpngs/universal-feature-update.git</t>
+  </si>
+  <si>
+    <t>9a2ae80c1ffa646c0829324b8bc02dfa5aa799c8</t>
   </si>
 </sst>
 </file>
@@ -411,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91329C54-249F-BC4E-96E0-56324FEC4D2F}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -435,6 +441,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changing the commit SHA
</commit_message>
<xml_diff>
--- a/feature_xlsx/1.0.0-example_feature/1.0.0-example_feature.xlsx
+++ b/feature_xlsx/1.0.0-example_feature/1.0.0-example_feature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nowpngs/Desktop/Programing/Personal/universal-feature-update/feature_xlsx/1.0.0-example_feature/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB9AAE5-DC64-B347-8D9D-BFFDAB733293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECECD75-0ABF-4B46-950F-E441EFF24020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2760" yWindow="1540" windowWidth="28040" windowHeight="17440" xr2:uid="{DDFCAD63-2E02-1143-AAA5-04CC48EE4CF7}"/>
   </bookViews>
@@ -50,7 +50,7 @@
     <t>git@github.com:Nowpngs/universal-feature-update.git</t>
   </si>
   <si>
-    <t>9a2ae80c1ffa646c0829324b8bc02dfa5aa799c8</t>
+    <t>7f75f22e0203c3636f2fddb170a310187631ce94</t>
   </si>
 </sst>
 </file>
@@ -420,7 +420,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>